<commit_message>
Updated memory excel sheet
</commit_message>
<xml_diff>
--- a/Soft RISC-V Memory Layout.xlsx
+++ b/Soft RISC-V Memory Layout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://purdue0-my.sharepoint.com/personal/pkaulkin_purdue_edu/Documents/2023-2024/Spring/ECET499/Labs/ECET499Soft Risc-V/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KjB22\Desktop\repos\soft-riscv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{94396EB9-A296-4835-958A-E82188CBC525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D640359F-BCAA-4710-B287-2F6ABEBF1521}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8A2B22-EB7E-41C2-B49F-BEDEC9E31292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{5EFF13C2-3DAD-4145-A748-59CDB3CFBC64}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{5EFF13C2-3DAD-4145-A748-59CDB3CFBC64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -173,10 +173,10 @@
     <t>0x200000</t>
   </si>
   <si>
-    <t>VGA BUF 2</t>
-  </si>
-  <si>
     <t>0xFFFF</t>
+  </si>
+  <si>
+    <t>VGA BUF 0</t>
   </si>
 </sst>
 </file>
@@ -585,18 +585,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F914173-28BE-41C0-BBE5-3EA32EBA6DE8}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E3" t="s">
         <v>2</v>
       </c>
@@ -604,7 +604,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
@@ -618,7 +618,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
@@ -632,7 +632,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
@@ -644,7 +644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
@@ -652,11 +652,11 @@
         <v>6</v>
       </c>
       <c r="J7">
-        <f t="shared" ref="J7:J37" si="0">J6+1</f>
+        <f t="shared" ref="J7:J36" si="0">J6+1</f>
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
@@ -668,7 +668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
@@ -680,7 +680,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
@@ -692,7 +692,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D11" s="1" t="s">
         <v>15</v>
       </c>
@@ -704,7 +704,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D12" s="1" t="s">
         <v>16</v>
       </c>
@@ -716,7 +716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D13" s="1" t="s">
         <v>27</v>
       </c>
@@ -728,7 +728,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D14" s="1" t="s">
         <v>28</v>
       </c>
@@ -740,7 +740,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D15" s="1" t="s">
         <v>29</v>
       </c>
@@ -752,7 +752,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D16" s="1" t="s">
         <v>30</v>
       </c>
@@ -764,7 +764,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D17" s="1" t="s">
         <v>31</v>
       </c>
@@ -776,7 +776,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D18" s="1" t="s">
         <v>32</v>
       </c>
@@ -788,7 +788,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D19" s="1" t="s">
         <v>33</v>
       </c>
@@ -800,7 +800,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D20" s="2" t="s">
         <v>34</v>
       </c>
@@ -812,7 +812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D21" s="2"/>
       <c r="E21" t="s">
         <v>18</v>
@@ -822,7 +822,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D22" s="2"/>
       <c r="E22" t="s">
         <v>18</v>
@@ -832,7 +832,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D23" s="2"/>
       <c r="E23" t="s">
         <v>18</v>
@@ -842,7 +842,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D24" s="2"/>
       <c r="E24" t="s">
         <v>19</v>
@@ -852,7 +852,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D25" s="3" t="s">
         <v>20</v>
       </c>
@@ -864,7 +864,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D26" s="3"/>
       <c r="E26" t="s">
         <v>18</v>
@@ -874,7 +874,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D27" s="3"/>
       <c r="E27" t="s">
         <v>18</v>
@@ -884,7 +884,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D28" s="3"/>
       <c r="E28" t="s">
         <v>18</v>
@@ -894,7 +894,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D29" s="3"/>
       <c r="E29" t="s">
         <v>18</v>
@@ -904,7 +904,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D30" s="3"/>
       <c r="E30" t="s">
         <v>25</v>
@@ -914,14 +914,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D31" s="4"/>
       <c r="J31">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D32" s="4"/>
       <c r="E32" t="s">
         <v>24</v>
@@ -931,7 +931,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D33" s="4"/>
       <c r="E33" t="s">
         <v>18</v>
@@ -941,7 +941,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D34" s="4"/>
       <c r="E34" t="s">
         <v>18</v>
@@ -951,9 +951,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D35" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E35" t="s">
         <v>23</v>
@@ -963,30 +963,30 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D36" s="5" t="s">
         <v>26</v>
       </c>
       <c r="E36" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="J36">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D37" s="5" t="s">
         <v>44</v>
       </c>
       <c r="E37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="38" spans="4:10" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D38" s="5"/>
     </row>
-    <row r="39" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D39" s="5" t="s">
         <v>21</v>
       </c>

</xml_diff>